<commit_message>
Image tags saving to database proof of concept.
</commit_message>
<xml_diff>
--- a/image_api_providers_comparasment.xlsx
+++ b/image_api_providers_comparasment.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simonas\Documents\c#\ImageTaggingApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simonas\Documents\c#\imgtag\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -338,10 +338,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -682,7 +682,7 @@
   <dimension ref="A2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +697,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -714,7 +714,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -729,7 +729,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -740,7 +740,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -755,7 +755,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
@@ -770,7 +770,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -800,7 +800,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -817,7 +817,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
@@ -832,7 +832,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -847,7 +847,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -862,7 +862,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -877,7 +877,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
@@ -892,7 +892,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
@@ -907,7 +907,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -922,161 +922,161 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="6"/>
@@ -1176,10 +1176,11 @@
     <hyperlink ref="E3" r:id="rId3"/>
     <hyperlink ref="A43" r:id="rId4" display="https://api.clarifai.com/v1/tag"/>
     <hyperlink ref="A44" r:id="rId5" display="https://api.clarifai.com/v1/tag/?model=general-v1.3"/>
+    <hyperlink ref="C4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>